<commit_message>
list of countries changed
</commit_message>
<xml_diff>
--- a/greta_summary.xlsx
+++ b/greta_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="33">
   <si>
     <t>height</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Luxembourg</t>
   </si>
   <si>
-    <t>Malta</t>
-  </si>
-  <si>
     <t>Norway</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
   </si>
   <si>
     <t>United Kingdom</t>
@@ -2207,16 +2207,16 @@
         <v>23</v>
       </c>
       <c r="C87">
-        <v>2180.162283360958</v>
+        <v>2275.731623768806</v>
       </c>
       <c r="D87">
-        <v>1780.868467748165</v>
+        <v>1416.522144913673</v>
       </c>
       <c r="E87">
-        <v>1621.067988872528</v>
+        <v>916.4812488555908</v>
       </c>
       <c r="F87">
-        <v>1481.775184869766</v>
+        <v>500.1176800131798</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2227,16 +2227,16 @@
         <v>23</v>
       </c>
       <c r="C88">
-        <v>2273.714855670929</v>
+        <v>2387.894743323326</v>
       </c>
       <c r="D88">
-        <v>1874.220068156719</v>
+        <v>1509.775882363319</v>
       </c>
       <c r="E88">
-        <v>1718.299560427666</v>
+        <v>989.4372624754906</v>
       </c>
       <c r="F88">
-        <v>1571.337879478931</v>
+        <v>548.6938955187798</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2247,16 +2247,16 @@
         <v>23</v>
       </c>
       <c r="C89">
-        <v>2353.032376468182</v>
+        <v>2494.119023442268</v>
       </c>
       <c r="D89">
-        <v>1962.385704755783</v>
+        <v>1597.215562164783</v>
       </c>
       <c r="E89">
-        <v>1804.07544618845</v>
+        <v>1059.242387652397</v>
       </c>
       <c r="F89">
-        <v>1652.03608995676</v>
+        <v>598.033249437809</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2267,16 +2267,16 @@
         <v>23</v>
       </c>
       <c r="C90">
-        <v>2431.7321844697</v>
+        <v>2591.285203576088</v>
       </c>
       <c r="D90">
-        <v>2041.219287633896</v>
+        <v>1682.66519588232</v>
       </c>
       <c r="E90">
-        <v>1883.586232066154</v>
+        <v>1124.612134039402</v>
       </c>
       <c r="F90">
-        <v>1730.918816506863</v>
+        <v>642.4829118847847</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2287,16 +2287,16 @@
         <v>23</v>
       </c>
       <c r="C91">
-        <v>2513.148107886314</v>
+        <v>2682.422887325287</v>
       </c>
       <c r="D91">
-        <v>2114.94973295927</v>
+        <v>1761.300552129745</v>
       </c>
       <c r="E91">
-        <v>1955.603492319584</v>
+        <v>1189.397022008896</v>
       </c>
       <c r="F91">
-        <v>1800.720677375793</v>
+        <v>687.306588947773</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2307,16 +2307,16 @@
         <v>24</v>
       </c>
       <c r="C92">
-        <v>2275.731623768806</v>
+        <v>2553.067083179951</v>
       </c>
       <c r="D92">
-        <v>1416.522144913673</v>
+        <v>2267.210143446922</v>
       </c>
       <c r="E92">
-        <v>916.4812488555908</v>
+        <v>2109.120178878307</v>
       </c>
       <c r="F92">
-        <v>500.1176800131798</v>
+        <v>1923.253001928329</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2327,16 +2327,16 @@
         <v>24</v>
       </c>
       <c r="C93">
-        <v>2387.894743323326</v>
+        <v>2717.374789535999</v>
       </c>
       <c r="D93">
-        <v>1509.775882363319</v>
+        <v>2420.792571425438</v>
       </c>
       <c r="E93">
-        <v>989.4372624754906</v>
+        <v>2252.09932333231</v>
       </c>
       <c r="F93">
-        <v>548.6938955187798</v>
+        <v>2059.990745961666</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2347,16 +2347,16 @@
         <v>24</v>
       </c>
       <c r="C94">
-        <v>2494.119023442268</v>
+        <v>2868.647428870201</v>
       </c>
       <c r="D94">
-        <v>1597.215562164783</v>
+        <v>2557.845230281353</v>
       </c>
       <c r="E94">
-        <v>1059.242387652397</v>
+        <v>2385.250291764736</v>
       </c>
       <c r="F94">
-        <v>598.033249437809</v>
+        <v>2187.971548318863</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2367,16 +2367,16 @@
         <v>24</v>
       </c>
       <c r="C95">
-        <v>2591.285203576088</v>
+        <v>3011.605755865574</v>
       </c>
       <c r="D95">
-        <v>1682.66519588232</v>
+        <v>2690.372838377953</v>
       </c>
       <c r="E95">
-        <v>1124.612134039402</v>
+        <v>2511.807695627213</v>
       </c>
       <c r="F95">
-        <v>642.4829118847847</v>
+        <v>2310.848719894886</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2387,16 +2387,16 @@
         <v>24</v>
       </c>
       <c r="C96">
-        <v>2682.422887325287</v>
+        <v>3143.178159475327</v>
       </c>
       <c r="D96">
-        <v>1761.300552129745</v>
+        <v>2815.456739008427</v>
       </c>
       <c r="E96">
-        <v>1189.397022008896</v>
+        <v>2631.745733737946</v>
       </c>
       <c r="F96">
-        <v>687.306588947773</v>
+        <v>2423.755839943886</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2407,16 +2407,16 @@
         <v>25</v>
       </c>
       <c r="C97">
-        <v>2553.067083179951</v>
+        <v>2002.66046667099</v>
       </c>
       <c r="D97">
-        <v>2267.210143446922</v>
+        <v>1522.391327857971</v>
       </c>
       <c r="E97">
-        <v>2109.120178878307</v>
+        <v>1205.881502747536</v>
       </c>
       <c r="F97">
-        <v>1923.253001928329</v>
+        <v>784.3784799575806</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2427,16 +2427,16 @@
         <v>25</v>
       </c>
       <c r="C98">
-        <v>2717.374789535999</v>
+        <v>2155.164343476295</v>
       </c>
       <c r="D98">
-        <v>2420.792571425438</v>
+        <v>1644.396299362183</v>
       </c>
       <c r="E98">
-        <v>2252.09932333231</v>
+        <v>1306.665119707584</v>
       </c>
       <c r="F98">
-        <v>2059.990745961666</v>
+        <v>857.9566776156425</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2447,16 +2447,16 @@
         <v>25</v>
       </c>
       <c r="C99">
-        <v>2868.647428870201</v>
+        <v>2293.333432435989</v>
       </c>
       <c r="D99">
-        <v>2557.845230281353</v>
+        <v>1756.850124239922</v>
       </c>
       <c r="E99">
-        <v>2385.250291764736</v>
+        <v>1405.096832871437</v>
       </c>
       <c r="F99">
-        <v>2187.971548318863</v>
+        <v>929.559429705143</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2467,16 +2467,16 @@
         <v>25</v>
       </c>
       <c r="C100">
-        <v>3011.605755865574</v>
+        <v>2426.06011068821</v>
       </c>
       <c r="D100">
-        <v>2690.372838377953</v>
+        <v>1864.987583935261</v>
       </c>
       <c r="E100">
-        <v>2511.807695627213</v>
+        <v>1496.18900758028</v>
       </c>
       <c r="F100">
-        <v>2310.848719894886</v>
+        <v>998.2617601156235</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2487,16 +2487,16 @@
         <v>25</v>
       </c>
       <c r="C101">
-        <v>3143.178159475327</v>
+        <v>2547.674983680248</v>
       </c>
       <c r="D101">
-        <v>2815.456739008427</v>
+        <v>1971.322158753872</v>
       </c>
       <c r="E101">
-        <v>2631.745733737946</v>
+        <v>1584.029371201992</v>
       </c>
       <c r="F101">
-        <v>2423.755839943886</v>
+        <v>1064.38362967968</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2507,16 +2507,16 @@
         <v>26</v>
       </c>
       <c r="C102">
-        <v>2002.66046667099</v>
+        <v>1305.225185334682</v>
       </c>
       <c r="D102">
-        <v>1522.391327857971</v>
+        <v>1006.473532557487</v>
       </c>
       <c r="E102">
-        <v>1205.881502747536</v>
+        <v>788.1479432582855</v>
       </c>
       <c r="F102">
-        <v>784.3784799575806</v>
+        <v>468.8485525250435</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2527,16 +2527,16 @@
         <v>26</v>
       </c>
       <c r="C103">
-        <v>2155.164343476295</v>
+        <v>1405.687756836414</v>
       </c>
       <c r="D103">
-        <v>1644.396299362183</v>
+        <v>1089.780430078506</v>
       </c>
       <c r="E103">
-        <v>1306.665119707584</v>
+        <v>859.0778263807297</v>
       </c>
       <c r="F103">
-        <v>857.9566776156425</v>
+        <v>515.3416250944138</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2547,16 +2547,16 @@
         <v>26</v>
       </c>
       <c r="C104">
-        <v>2293.333432435989</v>
+        <v>1497.511786818504</v>
       </c>
       <c r="D104">
-        <v>1756.850124239922</v>
+        <v>1168.922099471092</v>
       </c>
       <c r="E104">
-        <v>1405.096832871437</v>
+        <v>922.6750860214233</v>
       </c>
       <c r="F104">
-        <v>929.559429705143</v>
+        <v>560.5589485168457</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2567,16 +2567,16 @@
         <v>26</v>
       </c>
       <c r="C105">
-        <v>2426.06011068821</v>
+        <v>1589.794990897179</v>
       </c>
       <c r="D105">
-        <v>1864.987583935261</v>
+        <v>1244.538159966469</v>
       </c>
       <c r="E105">
-        <v>1496.18900758028</v>
+        <v>985.1509069800377</v>
       </c>
       <c r="F105">
-        <v>998.2617601156235</v>
+        <v>604.4192942976952</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2587,16 +2587,16 @@
         <v>26</v>
       </c>
       <c r="C106">
-        <v>2547.674983680248</v>
+        <v>1671.550665616989</v>
       </c>
       <c r="D106">
-        <v>1971.322158753872</v>
+        <v>1313.856243729591</v>
       </c>
       <c r="E106">
-        <v>1584.029371201992</v>
+        <v>1048.017984867096</v>
       </c>
       <c r="F106">
-        <v>1064.38362967968</v>
+        <v>646.8915796279907</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2607,16 +2607,16 @@
         <v>27</v>
       </c>
       <c r="C107">
-        <v>1305.225185334682</v>
+        <v>1861.892135977745</v>
       </c>
       <c r="D107">
-        <v>1006.473532557487</v>
+        <v>1341.936807453632</v>
       </c>
       <c r="E107">
-        <v>788.1479432582855</v>
+        <v>815.067846596241</v>
       </c>
       <c r="F107">
-        <v>468.8485525250435</v>
+        <v>429.3375449180603</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2627,16 +2627,16 @@
         <v>27</v>
       </c>
       <c r="C108">
-        <v>1405.687756836414</v>
+        <v>1991.727169930935</v>
       </c>
       <c r="D108">
-        <v>1089.780430078506</v>
+        <v>1449.705048859119</v>
       </c>
       <c r="E108">
-        <v>859.0778263807297</v>
+        <v>888.5665268301964</v>
       </c>
       <c r="F108">
-        <v>515.3416250944138</v>
+        <v>475.3643891215324</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2647,16 +2647,16 @@
         <v>27</v>
       </c>
       <c r="C109">
-        <v>1497.511786818504</v>
+        <v>2106.105921328068</v>
       </c>
       <c r="D109">
-        <v>1168.922099471092</v>
+        <v>1548.795731246471</v>
       </c>
       <c r="E109">
-        <v>922.6750860214233</v>
+        <v>959.5753737092018</v>
       </c>
       <c r="F109">
-        <v>560.5589485168457</v>
+        <v>518.1242534518242</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2667,16 +2667,16 @@
         <v>27</v>
       </c>
       <c r="C110">
-        <v>1589.794990897179</v>
+        <v>2214.934137761593</v>
       </c>
       <c r="D110">
-        <v>1244.538159966469</v>
+        <v>1641.76888769865</v>
       </c>
       <c r="E110">
-        <v>985.1509069800377</v>
+        <v>1027.779101192951</v>
       </c>
       <c r="F110">
-        <v>604.4192942976952</v>
+        <v>562.3006876707077</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2687,16 +2687,16 @@
         <v>27</v>
       </c>
       <c r="C111">
-        <v>1671.550665616989</v>
+        <v>2322.193554162979</v>
       </c>
       <c r="D111">
-        <v>1313.856243729591</v>
+        <v>1734.300208032131</v>
       </c>
       <c r="E111">
-        <v>1048.017984867096</v>
+        <v>1092.772762358189</v>
       </c>
       <c r="F111">
-        <v>646.8915796279907</v>
+        <v>604.6125956177711</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2707,16 +2707,16 @@
         <v>28</v>
       </c>
       <c r="C112">
-        <v>1861.892135977745</v>
+        <v>837.6263325810432</v>
       </c>
       <c r="D112">
-        <v>1341.936807453632</v>
+        <v>446.9185042381287</v>
       </c>
       <c r="E112">
-        <v>815.067846596241</v>
+        <v>189.232329249382</v>
       </c>
       <c r="F112">
-        <v>429.3375449180603</v>
+        <v>69.33625084161758</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2727,16 +2727,16 @@
         <v>28</v>
       </c>
       <c r="C113">
-        <v>1991.727169930935</v>
+        <v>908.7200992107391</v>
       </c>
       <c r="D113">
-        <v>1449.705048859119</v>
+        <v>493.9325910806656</v>
       </c>
       <c r="E113">
-        <v>888.5665268301964</v>
+        <v>213.5306243300438</v>
       </c>
       <c r="F113">
-        <v>475.3643891215324</v>
+        <v>80.08063733577728</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2747,16 +2747,16 @@
         <v>28</v>
       </c>
       <c r="C114">
-        <v>2106.105921328068</v>
+        <v>977.8934240341187</v>
       </c>
       <c r="D114">
-        <v>1548.795731246471</v>
+        <v>538.4895106554031</v>
       </c>
       <c r="E114">
-        <v>959.5753737092018</v>
+        <v>237.6326665878296</v>
       </c>
       <c r="F114">
-        <v>518.1242534518242</v>
+        <v>90.67244839668274</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2767,16 +2767,16 @@
         <v>28</v>
       </c>
       <c r="C115">
-        <v>2214.934137761593</v>
+        <v>1044.415025651455</v>
       </c>
       <c r="D115">
-        <v>1641.76888769865</v>
+        <v>582.3843482732773</v>
       </c>
       <c r="E115">
-        <v>1027.779101192951</v>
+        <v>261.2611892223358</v>
       </c>
       <c r="F115">
-        <v>562.3006876707077</v>
+        <v>101.5170537233353</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2787,16 +2787,16 @@
         <v>28</v>
       </c>
       <c r="C116">
-        <v>2322.193554162979</v>
+        <v>1108.767232954502</v>
       </c>
       <c r="D116">
-        <v>1734.300208032131</v>
+        <v>625.1524848341942</v>
       </c>
       <c r="E116">
-        <v>1092.772762358189</v>
+        <v>285.0623432993889</v>
       </c>
       <c r="F116">
-        <v>604.6125956177711</v>
+        <v>112.1650964617729</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2807,16 +2807,16 @@
         <v>29</v>
       </c>
       <c r="C117">
-        <v>837.6263325810432</v>
+        <v>2048.64157474041</v>
       </c>
       <c r="D117">
-        <v>446.9185042381287</v>
+        <v>1524.303337991238</v>
       </c>
       <c r="E117">
-        <v>189.232329249382</v>
+        <v>1188.391510486603</v>
       </c>
       <c r="F117">
-        <v>69.33625084161758</v>
+        <v>850.4308958053589</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2827,16 +2827,16 @@
         <v>29</v>
       </c>
       <c r="C118">
-        <v>908.7200992107391</v>
+        <v>2176.650778234005</v>
       </c>
       <c r="D118">
-        <v>493.9325910806656</v>
+        <v>1627.235871851444</v>
       </c>
       <c r="E118">
-        <v>213.5306243300438</v>
+        <v>1275.639413416386</v>
       </c>
       <c r="F118">
-        <v>80.08063733577728</v>
+        <v>918.0739293694496</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2847,16 +2847,16 @@
         <v>29</v>
       </c>
       <c r="C119">
-        <v>977.8934240341187</v>
+        <v>2291.032708525658</v>
       </c>
       <c r="D119">
-        <v>538.4895106554031</v>
+        <v>1720.019951224327</v>
       </c>
       <c r="E119">
-        <v>237.6326665878296</v>
+        <v>1354.343595862389</v>
       </c>
       <c r="F119">
-        <v>90.67244839668274</v>
+        <v>980.3375933170319</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2867,16 +2867,16 @@
         <v>29</v>
       </c>
       <c r="C120">
-        <v>1044.415025651455</v>
+        <v>2400.974631011486</v>
       </c>
       <c r="D120">
-        <v>582.3843482732773</v>
+        <v>1812.476114153862</v>
       </c>
       <c r="E120">
-        <v>261.2611892223358</v>
+        <v>1431.35782045126</v>
       </c>
       <c r="F120">
-        <v>101.5170537233353</v>
+        <v>1040.612736105919</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2887,16 +2887,16 @@
         <v>29</v>
       </c>
       <c r="C121">
-        <v>1108.767232954502</v>
+        <v>2504.189896166325</v>
       </c>
       <c r="D121">
-        <v>625.1524848341942</v>
+        <v>1895.440679788589</v>
       </c>
       <c r="E121">
-        <v>285.0623432993889</v>
+        <v>1501.442538499832</v>
       </c>
       <c r="F121">
-        <v>112.1650964617729</v>
+        <v>1098.305528759956</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2907,16 +2907,16 @@
         <v>30</v>
       </c>
       <c r="C122">
-        <v>2048.64157474041</v>
+        <v>1235.512368261814</v>
       </c>
       <c r="D122">
-        <v>1524.303337991238</v>
+        <v>662.7838175296783</v>
       </c>
       <c r="E122">
-        <v>1188.391510486603</v>
+        <v>493.5585297942162</v>
       </c>
       <c r="F122">
-        <v>850.4308958053589</v>
+        <v>375.9748919010162</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2927,16 +2927,16 @@
         <v>30</v>
       </c>
       <c r="C123">
-        <v>2176.650778234005</v>
+        <v>1325.299086153507</v>
       </c>
       <c r="D123">
-        <v>1627.235871851444</v>
+        <v>729.691873550415</v>
       </c>
       <c r="E123">
-        <v>1275.639413416386</v>
+        <v>548.583347260952</v>
       </c>
       <c r="F123">
-        <v>918.0739293694496</v>
+        <v>421.343171775341</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2947,16 +2947,16 @@
         <v>30</v>
       </c>
       <c r="C124">
-        <v>2291.032708525658</v>
+        <v>1410.358276546001</v>
       </c>
       <c r="D124">
-        <v>1720.019951224327</v>
+        <v>796.7720628380775</v>
       </c>
       <c r="E124">
-        <v>1354.343595862389</v>
+        <v>602.9315044879913</v>
       </c>
       <c r="F124">
-        <v>980.3375933170319</v>
+        <v>465.0983541607857</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2967,16 +2967,16 @@
         <v>30</v>
       </c>
       <c r="C125">
-        <v>2400.974631011486</v>
+        <v>1490.03730648756</v>
       </c>
       <c r="D125">
-        <v>1812.476114153862</v>
+        <v>858.0644109845161</v>
       </c>
       <c r="E125">
-        <v>1431.35782045126</v>
+        <v>654.7506504654884</v>
       </c>
       <c r="F125">
-        <v>1040.612736105919</v>
+        <v>507.2924704551697</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2987,16 +2987,16 @@
         <v>30</v>
       </c>
       <c r="C126">
-        <v>2504.189896166325</v>
+        <v>1567.997725248337</v>
       </c>
       <c r="D126">
-        <v>1895.440679788589</v>
+        <v>920.6912888288498</v>
       </c>
       <c r="E126">
-        <v>1501.442538499832</v>
+        <v>705.2688213586807</v>
       </c>
       <c r="F126">
-        <v>1098.305528759956</v>
+        <v>550.3703375458717</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3007,16 +3007,16 @@
         <v>31</v>
       </c>
       <c r="C127">
-        <v>1235.512368261814</v>
+        <v>1541.20716303587</v>
       </c>
       <c r="D127">
-        <v>662.7838175296783</v>
+        <v>998.7477750778198</v>
       </c>
       <c r="E127">
-        <v>493.5585297942162</v>
+        <v>715.1124797463417</v>
       </c>
       <c r="F127">
-        <v>375.9748919010162</v>
+        <v>353.2952439785004</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3027,16 +3027,16 @@
         <v>31</v>
       </c>
       <c r="C128">
-        <v>1325.299086153507</v>
+        <v>1635.944961965084</v>
       </c>
       <c r="D128">
-        <v>729.691873550415</v>
+        <v>1066.219932019711</v>
       </c>
       <c r="E128">
-        <v>548.583347260952</v>
+        <v>767.7444180846214</v>
       </c>
       <c r="F128">
-        <v>421.343171775341</v>
+        <v>380.2918564677238</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3047,16 +3047,16 @@
         <v>31</v>
       </c>
       <c r="C129">
-        <v>1410.358276546001</v>
+        <v>1722.925489604473</v>
       </c>
       <c r="D129">
-        <v>796.7720628380775</v>
+        <v>0</v>
       </c>
       <c r="E129">
-        <v>602.9315044879913</v>
+        <v>818.428347826004</v>
       </c>
       <c r="F129">
-        <v>465.0983541607857</v>
+        <v>406.4011368155479</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3067,16 +3067,16 @@
         <v>31</v>
       </c>
       <c r="C130">
-        <v>1490.03730648756</v>
+        <v>1804.89830738306</v>
       </c>
       <c r="D130">
-        <v>858.0644109845161</v>
+        <v>1192.588658511639</v>
       </c>
       <c r="E130">
-        <v>654.7506504654884</v>
+        <v>866.3668356537819</v>
       </c>
       <c r="F130">
-        <v>507.2924704551697</v>
+        <v>430.9836108088493</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3087,16 +3087,16 @@
         <v>31</v>
       </c>
       <c r="C131">
-        <v>1567.997725248337</v>
+        <v>1879.942884743214</v>
       </c>
       <c r="D131">
-        <v>920.6912888288498</v>
+        <v>1249.555326282978</v>
       </c>
       <c r="E131">
-        <v>705.2688213586807</v>
+        <v>912.3039106726646</v>
       </c>
       <c r="F131">
-        <v>550.3703375458717</v>
+        <v>454.9136902689934</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3206,7 +3206,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4280,16 +4280,16 @@
         <v>23</v>
       </c>
       <c r="C54">
-        <v>2183.274360199459</v>
+        <v>4335.09048619587</v>
       </c>
       <c r="D54">
-        <v>2108.514657133259</v>
+        <v>4278.155165070668</v>
       </c>
       <c r="E54">
-        <v>2108.514657133259</v>
+        <v>4239.306588788517</v>
       </c>
       <c r="F54">
-        <v>2108.514657133259</v>
+        <v>4168.334896015003</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -4300,16 +4300,16 @@
         <v>23</v>
       </c>
       <c r="C55">
-        <v>2266.625714551657</v>
+        <v>4474.823647866026</v>
       </c>
       <c r="D55">
-        <v>2190.054782411084</v>
+        <v>4411.306341225281</v>
       </c>
       <c r="E55">
-        <v>2190.054782411084</v>
+        <v>4369.454344303347</v>
       </c>
       <c r="F55">
-        <v>2190.054782411084</v>
+        <v>4299.289235630073</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -4320,16 +4320,16 @@
         <v>23</v>
       </c>
       <c r="C56">
-        <v>2300.902971817181</v>
+        <v>4533.564916032366</v>
       </c>
       <c r="D56">
-        <v>2224.761130847037</v>
+        <v>4468.890666681342</v>
       </c>
       <c r="E56">
-        <v>2224.761130847037</v>
+        <v>4422.495837335475</v>
       </c>
       <c r="F56">
-        <v>2224.761130847037</v>
+        <v>4355.946879304945</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -4340,16 +4340,16 @@
         <v>23</v>
       </c>
       <c r="C57">
-        <v>2363.180439835414</v>
+        <v>4633.606037246063</v>
       </c>
       <c r="D57">
-        <v>2285.904641808011</v>
+        <v>4567.249516957439</v>
       </c>
       <c r="E57">
-        <v>2285.904641808011</v>
+        <v>4511.886683093384</v>
       </c>
       <c r="F57">
-        <v>2285.904641808011</v>
+        <v>4449.841148620471</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -4360,16 +4360,16 @@
         <v>24</v>
       </c>
       <c r="C58">
-        <v>4335.09048619587</v>
+        <v>3701.378793229349</v>
       </c>
       <c r="D58">
-        <v>4278.155165070668</v>
+        <v>3515.83027680032</v>
       </c>
       <c r="E58">
-        <v>4239.306588788517</v>
+        <v>3453.867397326976</v>
       </c>
       <c r="F58">
-        <v>4168.334896015003</v>
+        <v>3381.020790426061</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -4380,16 +4380,16 @@
         <v>24</v>
       </c>
       <c r="C59">
-        <v>4474.823647866026</v>
+        <v>3835.900390129536</v>
       </c>
       <c r="D59">
-        <v>4411.306341225281</v>
+        <v>3649.958682899363</v>
       </c>
       <c r="E59">
-        <v>4369.454344303347</v>
+        <v>3588.844595178962</v>
       </c>
       <c r="F59">
-        <v>4299.289235630073</v>
+        <v>3510.00289837271</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4400,16 +4400,16 @@
         <v>24</v>
       </c>
       <c r="C60">
-        <v>4533.564916032366</v>
+        <v>3893.18142687995</v>
       </c>
       <c r="D60">
-        <v>4468.890666681342</v>
+        <v>3707.133432632312</v>
       </c>
       <c r="E60">
-        <v>4422.495837335475</v>
+        <v>3646.155625119805</v>
       </c>
       <c r="F60">
-        <v>4355.946879304945</v>
+        <v>3565.135307770222</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -4420,16 +4420,16 @@
         <v>24</v>
       </c>
       <c r="C61">
-        <v>4633.606037246063</v>
+        <v>3994.065821873955</v>
       </c>
       <c r="D61">
-        <v>4567.249516957439</v>
+        <v>3807.654034708627</v>
       </c>
       <c r="E61">
-        <v>4511.886683093384</v>
+        <v>3747.270229960792</v>
       </c>
       <c r="F61">
-        <v>4449.841148620471</v>
+        <v>3662.312051481567</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4440,16 +4440,16 @@
         <v>25</v>
       </c>
       <c r="C62">
-        <v>3701.378793229349</v>
+        <v>2777.376763748005</v>
       </c>
       <c r="D62">
-        <v>3515.83027680032</v>
+        <v>2777.376763748005</v>
       </c>
       <c r="E62">
-        <v>3453.867397326976</v>
+        <v>2777.376763748005</v>
       </c>
       <c r="F62">
-        <v>3381.020790426061</v>
+        <v>2724.513830953278</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -4460,16 +4460,16 @@
         <v>25</v>
       </c>
       <c r="C63">
-        <v>3835.900390129536</v>
+        <v>2889.373362679034</v>
       </c>
       <c r="D63">
-        <v>3649.958682899363</v>
+        <v>2889.373362679034</v>
       </c>
       <c r="E63">
-        <v>3588.844595178962</v>
+        <v>2889.373362679034</v>
       </c>
       <c r="F63">
-        <v>3510.00289837271</v>
+        <v>2832.764858206734</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -4480,16 +4480,16 @@
         <v>25</v>
       </c>
       <c r="C64">
-        <v>3893.18142687995</v>
+        <v>2937.29472562857</v>
       </c>
       <c r="D64">
-        <v>3707.133432632312</v>
+        <v>2937.29472562857</v>
       </c>
       <c r="E64">
-        <v>3646.155625119805</v>
+        <v>2937.29472562857</v>
       </c>
       <c r="F64">
-        <v>3565.135307770222</v>
+        <v>2877.968526558951</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -4500,16 +4500,16 @@
         <v>25</v>
       </c>
       <c r="C65">
-        <v>3994.065821873955</v>
+        <v>3021.516842307523</v>
       </c>
       <c r="D65">
-        <v>3807.654034708627</v>
+        <v>3021.516842307523</v>
       </c>
       <c r="E65">
-        <v>3747.270229960792</v>
+        <v>3021.516842307523</v>
       </c>
       <c r="F65">
-        <v>3662.312051481567</v>
+        <v>2959.571779896505</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4520,16 +4520,16 @@
         <v>26</v>
       </c>
       <c r="C66">
-        <v>2777.376763748005</v>
+        <v>1850.794092060067</v>
       </c>
       <c r="D66">
-        <v>2777.376763748005</v>
+        <v>1799.870604331605</v>
       </c>
       <c r="E66">
-        <v>2777.376763748005</v>
+        <v>1561.139701770619</v>
       </c>
       <c r="F66">
-        <v>2724.513830953278</v>
+        <v>1561.139701770619</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4540,16 +4540,16 @@
         <v>26</v>
       </c>
       <c r="C67">
-        <v>2889.373362679034</v>
+        <v>1947.245296792127</v>
       </c>
       <c r="D67">
-        <v>2889.373362679034</v>
+        <v>1898.815088885836</v>
       </c>
       <c r="E67">
-        <v>2889.373362679034</v>
+        <v>1649.881677495316</v>
       </c>
       <c r="F67">
-        <v>2832.764858206734</v>
+        <v>1649.881677495316</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4560,16 +4560,16 @@
         <v>26</v>
       </c>
       <c r="C68">
-        <v>2937.29472562857</v>
+        <v>1989.129211247899</v>
       </c>
       <c r="D68">
-        <v>2937.29472562857</v>
+        <v>1941.793102053925</v>
       </c>
       <c r="E68">
-        <v>2937.29472562857</v>
+        <v>1688.372960221022</v>
       </c>
       <c r="F68">
-        <v>2877.968526558951</v>
+        <v>1688.372960221022</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4580,16 +4580,16 @@
         <v>26</v>
       </c>
       <c r="C69">
-        <v>3021.516842307523</v>
+        <v>2064.701796034351</v>
       </c>
       <c r="D69">
-        <v>3021.516842307523</v>
+        <v>2018.605307576247</v>
       </c>
       <c r="E69">
-        <v>3021.516842307523</v>
+        <v>1757.645774805918</v>
       </c>
       <c r="F69">
-        <v>2959.571779896505</v>
+        <v>1757.645774805918</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4597,19 +4597,19 @@
         <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C70">
-        <v>1850.794092060067</v>
+        <v>902.9776683989912</v>
       </c>
       <c r="D70">
-        <v>1799.870604331605</v>
+        <v>902.9776683989912</v>
       </c>
       <c r="E70">
-        <v>1561.139701770619</v>
+        <v>902.9776683989912</v>
       </c>
       <c r="F70">
-        <v>1561.139701770619</v>
+        <v>902.9776683989912</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4617,19 +4617,19 @@
         <v>120</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C71">
-        <v>1947.245296792127</v>
+        <v>950.8296293001622</v>
       </c>
       <c r="D71">
-        <v>1898.815088885836</v>
+        <v>950.8296293001622</v>
       </c>
       <c r="E71">
-        <v>1649.881677495316</v>
+        <v>950.8296293001622</v>
       </c>
       <c r="F71">
-        <v>1649.881677495316</v>
+        <v>950.8296293001622</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4637,19 +4637,19 @@
         <v>130</v>
       </c>
       <c r="B72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C72">
-        <v>1989.129211247899</v>
+        <v>971.7057672319934</v>
       </c>
       <c r="D72">
-        <v>1941.793102053925</v>
+        <v>971.7057672319934</v>
       </c>
       <c r="E72">
-        <v>1688.372960221022</v>
+        <v>971.7057672319934</v>
       </c>
       <c r="F72">
-        <v>1688.372960221022</v>
+        <v>971.7057672319934</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4657,19 +4657,19 @@
         <v>150</v>
       </c>
       <c r="B73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C73">
-        <v>2064.701796034351</v>
+        <v>1009.349957607687</v>
       </c>
       <c r="D73">
-        <v>2018.605307576247</v>
+        <v>1009.349957607687</v>
       </c>
       <c r="E73">
-        <v>1757.645774805918</v>
+        <v>1009.349957607687</v>
       </c>
       <c r="F73">
-        <v>1757.645774805918</v>
+        <v>1009.349957607687</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4680,16 +4680,16 @@
         <v>29</v>
       </c>
       <c r="C74">
-        <v>902.9776683989912</v>
+        <v>2902.226679587737</v>
       </c>
       <c r="D74">
-        <v>902.9776683989912</v>
+        <v>2315.025327574462</v>
       </c>
       <c r="E74">
-        <v>902.9776683989912</v>
+        <v>1731.638803405687</v>
       </c>
       <c r="F74">
-        <v>902.9776683989912</v>
+        <v>1503.673371118493</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4700,16 +4700,16 @@
         <v>29</v>
       </c>
       <c r="C75">
-        <v>950.8296293001622</v>
+        <v>3004.297046642751</v>
       </c>
       <c r="D75">
-        <v>950.8296293001622</v>
+        <v>2400.058344172314</v>
       </c>
       <c r="E75">
-        <v>950.8296293001622</v>
+        <v>1825.298224644735</v>
       </c>
       <c r="F75">
-        <v>950.8296293001622</v>
+        <v>1582.986180850305</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4720,16 +4720,16 @@
         <v>29</v>
       </c>
       <c r="C76">
-        <v>971.7057672319934</v>
+        <v>3047.702262162231</v>
       </c>
       <c r="D76">
-        <v>971.7057672319934</v>
+        <v>2436.038276306354</v>
       </c>
       <c r="E76">
-        <v>971.7057672319934</v>
+        <v>1857.126806765795</v>
       </c>
       <c r="F76">
-        <v>971.7057672319934</v>
+        <v>1619.89783283975</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4740,16 +4740,16 @@
         <v>29</v>
       </c>
       <c r="C77">
-        <v>1009.349957607687</v>
+        <v>3122.031407553703</v>
       </c>
       <c r="D77">
-        <v>1009.349957607687</v>
+        <v>2499.419796512462</v>
       </c>
       <c r="E77">
-        <v>1009.349957607687</v>
+        <v>1913.742012614384</v>
       </c>
       <c r="F77">
-        <v>1009.349957607687</v>
+        <v>1668.775065403432</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4760,16 +4760,16 @@
         <v>30</v>
       </c>
       <c r="C78">
-        <v>2902.226679587737</v>
+        <v>3179.801477998495</v>
       </c>
       <c r="D78">
-        <v>2315.025327574462</v>
+        <v>2599.731954005547</v>
       </c>
       <c r="E78">
-        <v>1731.638803405687</v>
+        <v>2211.228871316649</v>
       </c>
       <c r="F78">
-        <v>1503.673371118493</v>
+        <v>1596.856395817362</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4780,16 +4780,16 @@
         <v>30</v>
       </c>
       <c r="C79">
-        <v>3004.297046642751</v>
+        <v>3308.987553254701</v>
       </c>
       <c r="D79">
-        <v>2400.058344172314</v>
+        <v>2725.773173653521</v>
       </c>
       <c r="E79">
-        <v>1825.298224644735</v>
+        <v>2319.355974745937</v>
       </c>
       <c r="F79">
-        <v>1582.986180850305</v>
+        <v>1676.531850663014</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -4800,16 +4800,16 @@
         <v>30</v>
       </c>
       <c r="C80">
-        <v>3047.702262162231</v>
+        <v>3363.165286182426</v>
       </c>
       <c r="D80">
-        <v>2436.038276306354</v>
+        <v>2780.207279570401</v>
       </c>
       <c r="E80">
-        <v>1857.126806765795</v>
+        <v>2365.753085954115</v>
       </c>
       <c r="F80">
-        <v>1619.89783283975</v>
+        <v>1710.866363768466</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4820,16 +4820,16 @@
         <v>30</v>
       </c>
       <c r="C81">
-        <v>3122.031407553703</v>
+        <v>3460.336588341743</v>
       </c>
       <c r="D81">
-        <v>2499.419796512462</v>
+        <v>2876.113258665428</v>
       </c>
       <c r="E81">
-        <v>1913.742012614384</v>
+        <v>2448.355136732571</v>
       </c>
       <c r="F81">
-        <v>1668.775065403432</v>
+        <v>1772.603532041423</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4837,19 +4837,19 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C82">
-        <v>3179.801477998495</v>
+        <v>4172.400136458687</v>
       </c>
       <c r="D82">
-        <v>2599.731954005547</v>
+        <v>3873.059447146021</v>
       </c>
       <c r="E82">
-        <v>2211.228871316649</v>
+        <v>3627.529885036871</v>
       </c>
       <c r="F82">
-        <v>1596.856395817362</v>
+        <v>3366.200209696777</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4857,19 +4857,19 @@
         <v>120</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C83">
-        <v>3308.987553254701</v>
+        <v>4284.974457044154</v>
       </c>
       <c r="D83">
-        <v>2725.773173653521</v>
+        <v>3991.497676415369</v>
       </c>
       <c r="E83">
-        <v>2319.355974745937</v>
+        <v>3738.809453439899</v>
       </c>
       <c r="F83">
-        <v>1676.531850663014</v>
+        <v>3475.440024910495</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4877,19 +4877,19 @@
         <v>130</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C84">
-        <v>3363.165286182426</v>
+        <v>4331.297058562748</v>
       </c>
       <c r="D84">
-        <v>2780.207279570401</v>
+        <v>4041.50435784366</v>
       </c>
       <c r="E84">
-        <v>2365.753085954115</v>
+        <v>3790.0902848728</v>
       </c>
       <c r="F84">
-        <v>1710.866363768466</v>
+        <v>3527.141216627322</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4897,98 +4897,18 @@
         <v>150</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C85">
-        <v>3460.336588341743</v>
+        <v>4417.843115345575</v>
       </c>
       <c r="D85">
-        <v>2876.113258665428</v>
+        <v>4123.537542345934</v>
       </c>
       <c r="E85">
-        <v>2448.355136732571</v>
+        <v>3878.943859986961</v>
       </c>
       <c r="F85">
-        <v>1772.603532041423</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86">
-        <v>100</v>
-      </c>
-      <c r="B86" t="s">
-        <v>32</v>
-      </c>
-      <c r="C86">
-        <v>4172.400136458687</v>
-      </c>
-      <c r="D86">
-        <v>3873.059447146021</v>
-      </c>
-      <c r="E86">
-        <v>3627.529885036871</v>
-      </c>
-      <c r="F86">
-        <v>3366.200209696777</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87">
-        <v>120</v>
-      </c>
-      <c r="B87" t="s">
-        <v>32</v>
-      </c>
-      <c r="C87">
-        <v>4284.974457044154</v>
-      </c>
-      <c r="D87">
-        <v>3991.497676415369</v>
-      </c>
-      <c r="E87">
-        <v>3738.809453439899</v>
-      </c>
-      <c r="F87">
-        <v>3475.440024910495</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88">
-        <v>130</v>
-      </c>
-      <c r="B88" t="s">
-        <v>32</v>
-      </c>
-      <c r="C88">
-        <v>4331.297058562748</v>
-      </c>
-      <c r="D88">
-        <v>4041.50435784366</v>
-      </c>
-      <c r="E88">
-        <v>3790.0902848728</v>
-      </c>
-      <c r="F88">
-        <v>3527.141216627322</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89">
-        <v>150</v>
-      </c>
-      <c r="B89" t="s">
-        <v>32</v>
-      </c>
-      <c r="C89">
-        <v>4417.843115345575</v>
-      </c>
-      <c r="D89">
-        <v>4123.537542345934</v>
-      </c>
-      <c r="E89">
-        <v>3878.943859986961</v>
-      </c>
-      <c r="F89">
         <v>3606.575570476241</v>
       </c>
     </row>
@@ -4999,7 +4919,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5279,7 +5199,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>800.1495496704625</v>
@@ -5296,7 +5216,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>1271.085173010904</v>
@@ -5313,7 +5233,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>1772.908122710768</v>
@@ -5330,7 +5250,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>1491.597543629729</v>
@@ -5347,7 +5267,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>1297.896930761573</v>
@@ -5364,7 +5284,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>1391.622585764305</v>
@@ -5381,7 +5301,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>2050.58263373399</v>
@@ -5398,7 +5318,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>909.4226664100015</v>
@@ -5415,18 +5335,35 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>1454.443934210046</v>
+      </c>
+      <c r="C25">
+        <v>1396.195655624956</v>
+      </c>
+      <c r="D25">
+        <v>1384.403167140272</v>
+      </c>
+      <c r="E25">
+        <v>1346.157242560637</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>1227.695325404156</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>1164.481464956607</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>1131.500707959445</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>1101.168220626289</v>
       </c>
     </row>
@@ -5754,16 +5691,16 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>1796.673188701752</v>
+        <v>928.8511360341778</v>
       </c>
       <c r="C19">
-        <v>1796.673188701752</v>
+        <v>813.2356794450787</v>
       </c>
       <c r="D19">
-        <v>1794.439365072262</v>
+        <v>736.1661932573647</v>
       </c>
       <c r="E19">
-        <v>1794.439365072262</v>
+        <v>655.7321918891065</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5771,16 +5708,16 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>928.8511360341778</v>
+        <v>1273.152363912779</v>
       </c>
       <c r="C20">
-        <v>813.2356794450787</v>
+        <v>1248.929234338325</v>
       </c>
       <c r="D20">
-        <v>736.1661932573647</v>
+        <v>1227.586790957984</v>
       </c>
       <c r="E20">
-        <v>655.7321918891065</v>
+        <v>1183.930689575113</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5788,16 +5725,16 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>1273.152363912779</v>
+        <v>1818.581508355931</v>
       </c>
       <c r="C21">
-        <v>1248.929234338325</v>
+        <v>1713.801094327607</v>
       </c>
       <c r="D21">
-        <v>1227.586790957984</v>
+        <v>1663.952030782774</v>
       </c>
       <c r="E21">
-        <v>1183.930689575113</v>
+        <v>1653.6661088541</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5805,16 +5742,16 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>1818.581508355931</v>
+        <v>1444.037472513454</v>
       </c>
       <c r="C22">
-        <v>1713.801094327607</v>
+        <v>1417.965512498977</v>
       </c>
       <c r="D22">
-        <v>1663.952030782774</v>
+        <v>1388.728657984853</v>
       </c>
       <c r="E22">
-        <v>1653.6661088541</v>
+        <v>1368.602387990994</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5822,16 +5759,16 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>1444.037472513454</v>
+        <v>1325.542640048631</v>
       </c>
       <c r="C23">
-        <v>1417.965512498977</v>
+        <v>1304.553611041183</v>
       </c>
       <c r="D23">
-        <v>1388.728657984853</v>
+        <v>1295.687960327162</v>
       </c>
       <c r="E23">
-        <v>1368.602387990994</v>
+        <v>1291.849458097553</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5839,16 +5776,16 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>1325.542640048631</v>
+        <v>1380.561294203357</v>
       </c>
       <c r="C24">
-        <v>1304.553611041183</v>
+        <v>1380.175089558726</v>
       </c>
       <c r="D24">
-        <v>1295.687960327162</v>
+        <v>1371.175406295972</v>
       </c>
       <c r="E24">
-        <v>1291.849458097553</v>
+        <v>1355.881190350131</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5856,16 +5793,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>1380.561294203357</v>
+        <v>1859.949632086058</v>
       </c>
       <c r="C25">
-        <v>1380.175089558726</v>
+        <v>1793.901102114377</v>
       </c>
       <c r="D25">
-        <v>1371.175406295972</v>
+        <v>1761.415185498268</v>
       </c>
       <c r="E25">
-        <v>1355.881190350131</v>
+        <v>1722.760394453647</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5873,16 +5810,16 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>1859.949632086058</v>
+        <v>1041.262890381925</v>
       </c>
       <c r="C26">
-        <v>1793.901102114377</v>
+        <v>891.5881328343361</v>
       </c>
       <c r="D26">
-        <v>1761.415185498268</v>
+        <v>848.1697540724834</v>
       </c>
       <c r="E26">
-        <v>1722.760394453647</v>
+        <v>807.1292256336436</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5890,16 +5827,16 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>1041.262890381925</v>
+        <v>1483.457073051132</v>
       </c>
       <c r="C27">
-        <v>891.5881328343361</v>
+        <v>1384.403167140272</v>
       </c>
       <c r="D27">
-        <v>848.1697540724834</v>
+        <v>1379.782715489062</v>
       </c>
       <c r="E27">
-        <v>807.1292256336436</v>
+        <v>1346.157242560637</v>
       </c>
     </row>
     <row r="28" spans="1:5">

</xml_diff>